<commit_message>
Clean and reshuffle evaluation Dataset
</commit_message>
<xml_diff>
--- a/docs/table-data(Api)2.xlsx
+++ b/docs/table-data(Api)2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="28220"/>
+    <workbookView windowHeight="18160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1802,7 +1802,7 @@
     <t xml:space="preserve">Start a cubic basis spline motion command in which the spline is traversed using a motion profile. The point positions are specified as absolute positions. </t>
   </si>
   <si>
-    <t xml:space="preserve"> StartCBSplinePos(int channel, VelAccLimitedSplineCommand *pSplineCommand, unsigned int numPoints, SplinePoint *pPoint) </t>
+    <t xml:space="preserve">StartCBSplinePos(int channel, VelAccLimitedSplineCommand *pSplineCommand, unsigned int numPoints, SplinePoint *pPoint) </t>
   </si>
   <si>
     <t>Start a cubic basis spline motion command in which the spline is traversed while staying within the specified velocity and acceleration limits for each axis. The point positions are specified as absolute positions.</t>
@@ -1820,7 +1820,7 @@
     <t>Start a cubic basis spline motion command in which the total time to complete the spline is specified. The point positions are specified as relative positions.</t>
   </si>
   <si>
-    <t xml:space="preserve">StartCBSplineMov(int channel, ProfileSplineCommand *pSplineCommand, unsigned int numPoints, SplinePoint *pPoint) </t>
+    <t>StartCBSplineMov(int channel, ProfileSplineCommand *pSplineCommand, unsigned int numPoints, SplinePoint *pPoint)</t>
   </si>
   <si>
     <t>Start a cubic basis spline motion command in which the spline is traversed using a motion profile. The point positions are specified as relative positions.</t>
@@ -6948,7 +6948,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6959,13 +6959,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -7433,28 +7426,31 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -7463,118 +7459,115 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -7931,14 +7924,14 @@
   <sheetPr/>
   <dimension ref="A1:D1376"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" topLeftCell="C1219" workbookViewId="0">
+      <selection activeCell="C1265" sqref="C1265"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="11.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="117.857142857143" customWidth="1"/>
+    <col min="2" max="2" width="182.607142857143" customWidth="1"/>
     <col min="3" max="3" width="255.642857142857" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>